<commit_message>
More Plots using qplots, qqplots, lattice plots
</commit_message>
<xml_diff>
--- a/doc/Summary Stats.xlsx
+++ b/doc/Summary Stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="16275" windowHeight="8250" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="16275" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="loansRaw" sheetId="1" r:id="rId1"/>
@@ -404,8 +404,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -468,9 +468,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -487,13 +484,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +524,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -805,11 +804,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="43435008"/>
-        <c:axId val="43494784"/>
+        <c:axId val="1019051520"/>
+        <c:axId val="537701760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43435008"/>
+        <c:axId val="1019051520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +817,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43494784"/>
+        <c:crossAx val="537701760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -826,7 +825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43494784"/>
+        <c:axId val="537701760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,14 +841,13 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="43435008"/>
+        <c:crossAx val="1019051520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1217,69 +1215,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="1">
         <v>1000</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D3">
         <v>-0.01</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J3">
@@ -1287,31 +1285,31 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>6000</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D4">
         <v>6000</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F4">
         <v>7</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="1">
         <v>5586</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="J4">
@@ -1319,31 +1317,31 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="1">
         <v>10000</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D5">
         <v>10000</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F5">
         <v>9</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="1">
         <v>10962</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="J5">
@@ -1351,31 +1349,31 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="1">
         <v>12406</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D6">
         <v>12001.57</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F6">
         <v>10.08</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="1">
         <v>15245</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="J6">
@@ -1383,31 +1381,31 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>17000</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D7">
         <v>16000</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F7">
         <v>13</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="1">
         <v>18889</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J7">
@@ -1415,31 +1413,31 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="1">
         <v>35000</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D8">
         <v>35000</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F8">
         <v>38</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H8" s="1">
         <v>270800</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="J8">
@@ -1447,33 +1445,33 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B9" s="1">
         <f>+B8-B3</f>
         <v>34000</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="1">
         <f>+D8-D3</f>
         <v>35000.01</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="1">
         <v>2</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="J9">
@@ -1481,21 +1479,21 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>57</v>
       </c>
       <c r="F10" s="1">
         <f>+F8-F3</f>
         <v>36</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>57</v>
       </c>
       <c r="H10" s="1">
         <f>+H8-H3</f>
         <v>270800</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J10" s="1">
@@ -2052,11 +2050,11 @@
     <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2118,7 +2116,7 @@
       <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="14">
         <v>0</v>
       </c>
     </row>
@@ -2150,7 +2148,7 @@
       <c r="I5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="14">
         <v>0</v>
       </c>
     </row>
@@ -2182,7 +2180,7 @@
       <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="14">
         <v>0</v>
       </c>
     </row>
@@ -2214,7 +2212,7 @@
       <c r="I7" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="14">
         <v>0.90129999999999999</v>
       </c>
     </row>
@@ -2246,7 +2244,7 @@
       <c r="I8" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="14">
         <v>1</v>
       </c>
     </row>
@@ -2278,7 +2276,7 @@
       <c r="I9" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="14">
         <v>9</v>
       </c>
     </row>
@@ -2312,7 +2310,7 @@
       <c r="I10" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="14">
         <v>2</v>
       </c>
     </row>
@@ -2348,58 +2346,58 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.1212</v>
       </c>
       <c r="B13">
         <v>122</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="12">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="B14">
         <v>119</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="A15" s="12">
         <v>0.13109999999999999</v>
       </c>
       <c r="B15">
         <v>115</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16" s="12">
         <v>0.15310000000000001</v>
       </c>
       <c r="B16">
         <v>76</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="A17" s="13">
         <v>0.1409</v>
       </c>
       <c r="B17" s="1">
         <v>72</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="A18" s="13">
         <v>0.14330000000000001</v>
       </c>
       <c r="B18" s="1">
         <v>69</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -2408,7 +2406,7 @@
       <c r="B19" s="1">
         <v>1927</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -2517,7 +2515,7 @@
       <c r="B35">
         <v>8</v>
       </c>
-      <c r="C35" s="11"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -2526,7 +2524,7 @@
       <c r="B36">
         <v>6</v>
       </c>
-      <c r="C36" s="11"/>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
@@ -2535,7 +2533,7 @@
       <c r="B37">
         <v>5</v>
       </c>
-      <c r="C37" s="11"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
@@ -2544,7 +2542,7 @@
       <c r="B38">
         <v>5</v>
       </c>
-      <c r="C38" s="11"/>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -2553,7 +2551,7 @@
       <c r="B39">
         <v>5</v>
       </c>
-      <c r="C39" s="11"/>
+      <c r="C39" s="10"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -2562,7 +2560,7 @@
       <c r="B40">
         <v>5</v>
       </c>
-      <c r="C40" s="11"/>
+      <c r="C40" s="10"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -2571,7 +2569,7 @@
       <c r="B41">
         <v>2466</v>
       </c>
-      <c r="C41" s="11"/>
+      <c r="C41" s="10"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -2700,7 +2698,7 @@
       <c r="B60">
         <v>588.5</v>
       </c>
-      <c r="C60" s="10"/>
+      <c r="C60" s="9"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -2709,7 +2707,7 @@
       <c r="B61">
         <v>3500</v>
       </c>
-      <c r="C61" s="10"/>
+      <c r="C61" s="9"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -2718,7 +2716,7 @@
       <c r="B62">
         <v>5000</v>
       </c>
-      <c r="C62" s="10"/>
+      <c r="C62" s="9"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -2727,7 +2725,7 @@
       <c r="B63">
         <v>5688.9</v>
       </c>
-      <c r="C63" s="10"/>
+      <c r="C63" s="9"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -2736,7 +2734,7 @@
       <c r="B64">
         <v>6800</v>
       </c>
-      <c r="C64" s="10"/>
+      <c r="C64" s="9"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -2745,7 +2743,7 @@
       <c r="B65">
         <v>102750</v>
       </c>
-      <c r="C65" s="10"/>
+      <c r="C65" s="9"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
@@ -2754,7 +2752,7 @@
       <c r="B66">
         <v>1</v>
       </c>
-      <c r="C66" s="10"/>
+      <c r="C66" s="9"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
@@ -2893,8 +2891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3133,7 +3131,7 @@
       <c r="C16" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3163,7 +3161,7 @@
       <c r="C18" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3208,7 +3206,7 @@
       <c r="C21" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3290,7 +3288,7 @@
       <c r="B3" s="1">
         <v>5</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <f>+B3/$B$41</f>
         <v>2E-3</v>
       </c>
@@ -3302,7 +3300,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <f t="shared" ref="C4:C40" si="0">+B4/$B$41</f>
         <v>1.1999999999999999E-3</v>
       </c>
@@ -3314,7 +3312,7 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <f t="shared" si="0"/>
         <v>4.0000000000000002E-4</v>
       </c>
@@ -3326,7 +3324,7 @@
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <f t="shared" si="0"/>
         <v>1.6000000000000001E-3</v>
       </c>
@@ -3338,7 +3336,7 @@
       <c r="B7">
         <v>125</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
@@ -3350,7 +3348,7 @@
       <c r="B8">
         <v>145</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <f t="shared" si="0"/>
         <v>5.8000000000000003E-2</v>
       </c>
@@ -3362,7 +3360,7 @@
       <c r="B9">
         <v>171</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <f t="shared" si="0"/>
         <v>6.8400000000000002E-2</v>
       </c>
@@ -3374,7 +3372,7 @@
       <c r="B10">
         <v>166</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <f t="shared" si="0"/>
         <v>6.6400000000000001E-2</v>
       </c>
@@ -3386,7 +3384,7 @@
       <c r="B11">
         <v>157</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <f t="shared" si="0"/>
         <v>6.2799999999999995E-2</v>
       </c>
@@ -3398,7 +3396,7 @@
       <c r="B12">
         <v>138</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <f t="shared" si="0"/>
         <v>5.5199999999999999E-2</v>
       </c>
@@ -3410,7 +3408,7 @@
       <c r="B13">
         <v>140</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <f t="shared" si="0"/>
         <v>5.6000000000000001E-2</v>
       </c>
@@ -3422,7 +3420,7 @@
       <c r="B14">
         <v>153</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <f t="shared" si="0"/>
         <v>6.1199999999999997E-2</v>
       </c>
@@ -3434,7 +3432,7 @@
       <c r="B15">
         <v>131</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <f t="shared" si="0"/>
         <v>5.2400000000000002E-2</v>
       </c>
@@ -3446,7 +3444,7 @@
       <c r="B16" s="1">
         <v>134</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <f t="shared" si="0"/>
         <v>5.3600000000000002E-2</v>
       </c>
@@ -3458,7 +3456,7 @@
       <c r="B17">
         <v>112</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <f t="shared" si="0"/>
         <v>4.48E-2</v>
       </c>
@@ -3470,7 +3468,7 @@
       <c r="B18">
         <v>93</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <f t="shared" si="0"/>
         <v>3.7199999999999997E-2</v>
       </c>
@@ -3482,7 +3480,7 @@
       <c r="B19">
         <v>114</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <f t="shared" si="0"/>
         <v>4.5600000000000002E-2</v>
       </c>
@@ -3494,7 +3492,7 @@
       <c r="B20">
         <v>94</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="11">
         <f t="shared" si="0"/>
         <v>3.7600000000000001E-2</v>
       </c>
@@ -3506,7 +3504,7 @@
       <c r="B21">
         <v>94</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <f t="shared" si="0"/>
         <v>3.7600000000000001E-2</v>
       </c>
@@ -3518,7 +3516,7 @@
       <c r="B22">
         <v>65</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <f t="shared" si="0"/>
         <v>2.5999999999999999E-2</v>
       </c>
@@ -3530,7 +3528,7 @@
       <c r="B23">
         <v>53</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <f t="shared" si="0"/>
         <v>2.12E-2</v>
       </c>
@@ -3542,7 +3540,7 @@
       <c r="B24">
         <v>54</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="11">
         <f t="shared" si="0"/>
         <v>2.1600000000000001E-2</v>
       </c>
@@ -3554,7 +3552,7 @@
       <c r="B25">
         <v>61</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="11">
         <f t="shared" si="0"/>
         <v>2.4400000000000002E-2</v>
       </c>
@@ -3566,7 +3564,7 @@
       <c r="B26">
         <v>46</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <f t="shared" si="0"/>
         <v>1.84E-2</v>
       </c>
@@ -3578,7 +3576,7 @@
       <c r="B27">
         <v>46</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="11">
         <f t="shared" si="0"/>
         <v>1.84E-2</v>
       </c>
@@ -3590,7 +3588,7 @@
       <c r="B28">
         <v>36</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="11">
         <f t="shared" si="0"/>
         <v>1.44E-2</v>
       </c>
@@ -3602,7 +3600,7 @@
       <c r="B29" s="1">
         <v>17</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="11">
         <f t="shared" si="0"/>
         <v>6.7999999999999996E-3</v>
       </c>
@@ -3614,7 +3612,7 @@
       <c r="B30">
         <v>22</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="11">
         <f t="shared" si="0"/>
         <v>8.8000000000000005E-3</v>
       </c>
@@ -3626,7 +3624,7 @@
       <c r="B31">
         <v>28</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="11">
         <f t="shared" si="0"/>
         <v>1.12E-2</v>
       </c>
@@ -3638,7 +3636,7 @@
       <c r="B32">
         <v>19</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="11">
         <f t="shared" si="0"/>
         <v>7.6E-3</v>
       </c>
@@ -3650,7 +3648,7 @@
       <c r="B33">
         <v>20</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="11">
         <f t="shared" si="0"/>
         <v>8.0000000000000002E-3</v>
       </c>
@@ -3662,7 +3660,7 @@
       <c r="B34">
         <v>13</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="11">
         <f t="shared" si="0"/>
         <v>5.1999999999999998E-3</v>
       </c>
@@ -3674,7 +3672,7 @@
       <c r="B35">
         <v>13</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="11">
         <f t="shared" si="0"/>
         <v>5.1999999999999998E-3</v>
       </c>
@@ -3686,7 +3684,7 @@
       <c r="B36">
         <v>11</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="11">
         <f t="shared" si="0"/>
         <v>4.4000000000000003E-3</v>
       </c>
@@ -3698,7 +3696,7 @@
       <c r="B37">
         <v>8</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="11">
         <f t="shared" si="0"/>
         <v>3.2000000000000002E-3</v>
       </c>
@@ -3710,7 +3708,7 @@
       <c r="B38">
         <v>6</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="11">
         <f t="shared" si="0"/>
         <v>2.3999999999999998E-3</v>
       </c>
@@ -3722,7 +3720,7 @@
       <c r="B39">
         <v>1</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="11">
         <f t="shared" si="0"/>
         <v>4.0000000000000002E-4</v>
       </c>
@@ -3734,7 +3732,7 @@
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C40" s="11">
         <f t="shared" si="0"/>
         <v>4.0000000000000002E-4</v>
       </c>
@@ -3747,7 +3745,7 @@
         <f>SUM(B3:B40)</f>
         <v>2500</v>
       </c>
-      <c r="C41" s="16">
+      <c r="C41" s="15">
         <f>SUM(C3:C40)</f>
         <v>0.99999999999999956</v>
       </c>

</xml_diff>